<commit_message>
Update Small Things in Playbooks for Metric Parser
Update a couple of small things in the Playbook Metric generator example
playbooks.
</commit_message>
<xml_diff>
--- a/python--deployment-metric-parser/examples/Playbook_3.xlsx
+++ b/python--deployment-metric-parser/examples/Playbook_3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32800" yWindow="19060" windowWidth="33000" windowHeight="14540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-33000" yWindow="460" windowWidth="33000" windowHeight="14540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -842,7 +842,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,7 +1318,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Meta!$A$2:$A$5</xm:f>
@@ -1336,7 +1336,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>